<commit_message>
Added Board Name, fixed File Check Errors from 4PCB, Renamed Output Job File to MainOutputs.OutJob
</commit_message>
<xml_diff>
--- a/UL-SWAP-DAQ-1/Project Outputs for UL-SWAP-DAQ-2/BOM/ULSWAPDAQ2-BOM-UL-SWAP-DAQ-2.xlsx
+++ b/UL-SWAP-DAQ-1/Project Outputs for UL-SWAP-DAQ-2/BOM/ULSWAPDAQ2-BOM-UL-SWAP-DAQ-2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brea McWhirter\Desktop\ULSWAPDAQ\ULSWAPDAQ\UL-SWAP-DAQ-1\Project Outputs for UL-SWAP-DAQ-2\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29E22D41-DFA9-4D83-B637-D90462599B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{863BE3F5-91D0-482E-9E54-4E8A857FE404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10545" yWindow="1560" windowWidth="38700" windowHeight="15375" xr2:uid="{76CCECDD-185A-4B50-BC46-5065D9FF7DC3}"/>
+    <workbookView xWindow="10545" yWindow="1560" windowWidth="38700" windowHeight="15375" xr2:uid="{241EC38D-7FB0-485B-B2B5-178DC0E3ECE4}"/>
   </bookViews>
   <sheets>
     <sheet name="ULSWAPDAQ2-BOM-UL-SWAP-DAQ-2" sheetId="1" r:id="rId1"/>
@@ -1192,7 +1192,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34EED3A-5641-45C6-86A3-279B2A437038}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E0BB1B9-38A9-41A1-956D-B223C6855D41}">
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Final BOM edits, no major changes.
</commit_message>
<xml_diff>
--- a/UL-SWAP-DAQ-1/Project Outputs for UL-SWAP-DAQ-2/BOM/ULSWAPDAQ2-BOM-UL-SWAP-DAQ-2.xlsx
+++ b/UL-SWAP-DAQ-1/Project Outputs for UL-SWAP-DAQ-2/BOM/ULSWAPDAQ2-BOM-UL-SWAP-DAQ-2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abain\Desktop\ULSWAPDAQ\UL-SWAP-DAQ-1\Project Outputs for UL-SWAP-DAQ-2\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEF9E34A-E284-4621-B34F-8341082F3F7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B5A3B9B-2D74-4D12-8EA4-DCF9DCFD62B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="8680" xr2:uid="{82143A8C-7AE0-4845-81EA-21E0151BD428}"/>
+    <workbookView xWindow="340" yWindow="340" windowWidth="14400" windowHeight="8680" xr2:uid="{E0BEAD89-D4A9-4850-841A-4E1E73F269A8}"/>
   </bookViews>
   <sheets>
     <sheet name="ULSWAPDAQ2-BOM-UL-SWAP-DAQ-2" sheetId="1" r:id="rId1"/>
@@ -949,7 +949,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4433E244-3DA0-4C99-8528-C0AB48894D7C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73524877-ACFA-4B96-AD85-D62DA367FFA1}">
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>